<commit_message>
Fri Jan  6 10:59:11 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2022鸡丁计划.xlsx
+++ b/计划/2022鸡丁计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="13180" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="鸡丁个人档案" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
   <si>
     <t>已获得成就</t>
   </si>
@@ -71,22 +71,22 @@
     <t>熟练背会10首唐诗</t>
   </si>
   <si>
-    <t>12月第2周</t>
-  </si>
-  <si>
-    <t>2022.12.5</t>
-  </si>
-  <si>
-    <t>2022.12.6</t>
-  </si>
-  <si>
-    <t>2022.12.7</t>
-  </si>
-  <si>
-    <t>2022.12.8</t>
-  </si>
-  <si>
-    <t>2022.12.9</t>
+    <t>12月第3周</t>
+  </si>
+  <si>
+    <t>2022.12.12</t>
+  </si>
+  <si>
+    <t>2022.12.13</t>
+  </si>
+  <si>
+    <t>2022.12.14</t>
+  </si>
+  <si>
+    <t>2022.12.15</t>
+  </si>
+  <si>
+    <t>2022.12.16</t>
   </si>
   <si>
     <t>汉字</t>
@@ -99,7 +99,7 @@
   </si>
   <si>
     <t>1. 读一遍乘法表
-2. 背一遍 6 以内乘法表</t>
+2. 背一遍 7 以内乘法表</t>
   </si>
   <si>
     <t>看书</t>
@@ -112,19 +112,22 @@
     <t>锻炼</t>
   </si>
   <si>
+    <t>篮球</t>
+  </si>
+  <si>
     <t>跳高</t>
   </si>
   <si>
     <t>积分</t>
   </si>
   <si>
-    <t>⭐️</t>
-  </si>
-  <si>
-    <t>2022.12.10</t>
-  </si>
-  <si>
-    <t>2022.12.11</t>
+    <t>☆</t>
+  </si>
+  <si>
+    <t>2022.12.17</t>
+  </si>
+  <si>
+    <t>2022.12.18</t>
   </si>
 </sst>
 </file>
@@ -132,10 +135,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -161,24 +164,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,46 +211,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,11 +226,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -267,6 +278,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -274,32 +293,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,19 +329,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,31 +467,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,127 +503,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,6 +538,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -546,6 +582,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -565,21 +616,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -594,41 +630,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -637,152 +640,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -800,9 +803,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1152,90 +1152,90 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.703125" defaultRowHeight="40" customHeight="1" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="16382" width="23.703125" style="11" customWidth="1"/>
+    <col min="1" max="16382" width="23.703125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="D2" s="13" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="D3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="D4" s="13" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="D6" s="13" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="D7" s="13" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="D7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="D8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1252,7 +1252,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -1347,48 +1347,48 @@
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="2:3">
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" customHeight="1" spans="1:3">
@@ -1429,30 +1429,30 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>